<commit_message>
Control and top Practica_A2
</commit_message>
<xml_diff>
--- a/Practica_A2/Planificación (tabla de reserva).xlsx
+++ b/Practica_A2/Planificación (tabla de reserva).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos_vivado\ADAV\Practica_A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269E6851-B000-4EA3-B1F2-922393B3C73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56C0EAC-5323-45FF-85B2-96A70F459783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{3D0D9D7F-F8C4-4ECB-BEE3-D3B5C4F2AAF5}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{3D0D9D7F-F8C4-4ECB-BEE3-D3B5C4F2AAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Primera_Simplificación" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="92">
   <si>
     <t>Multiplicador</t>
   </si>
@@ -246,33 +246,12 @@
     <t>Vida del registro -&gt;</t>
   </si>
   <si>
-    <t>Cambio de orden de ejucuión de tmp6 -&gt; tmp9 (inverttido)</t>
-  </si>
-  <si>
     <t>4º Tabla de reserva</t>
   </si>
   <si>
     <t>5º Agrupar operaciones</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>Uso de datos -&gt;</t>
   </si>
   <si>
@@ -280,6 +259,86 @@
   </si>
   <si>
     <t>No se puede leer en el mismo cilco en el que se ha realizado la escritura del registro hay que esperar al siguiente ciclo.</t>
+  </si>
+  <si>
+    <t>Cambio de orden de ejucuión de tmp6 -&gt; tmp9 (invertido)</t>
+  </si>
+  <si>
+    <t>Numero mínimo de registros -&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El número mínimo de registros es igual al máximo número de  X en cualquier fila de la paralelización </t>
+  </si>
+  <si>
+    <t>Tabla de reserva</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>r4</t>
+  </si>
+  <si>
+    <t>r5</t>
+  </si>
+  <si>
+    <t>r6</t>
+  </si>
+  <si>
+    <t>Primera aproximación</t>
+  </si>
+  <si>
+    <t>Segunda aproximaxión -&gt; r1: tmp14, tmp18 &lt;-&gt; r4: tmp17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Carga de datos finales en operaciones inicales</t>
+  </si>
+  <si>
+    <t>tmp15 -&gt; sv4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmp16 -&gt; sv3 </t>
+  </si>
+  <si>
+    <t>tmp17 -&gt; sv2</t>
+  </si>
+  <si>
+    <t>tmp18 -&gt; sv1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Esta configuración es mejor en sobreescritura de registros. Se debe a que nos ahoramos hacer cambios de más entre registros, que es lo que sucedería si cambiamos  r1: tmp14, tmp18 &lt;-&gt; r4: tmp17. Esto provocaría que el  intercambio de información no sea solamente los registros r1 y r3, sino que también involucraríamos a r4. Por lo que elegiré la </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>primera aproximación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -483,7 +542,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -506,6 +565,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -513,7 +669,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,11 +741,67 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -939,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD72D291-E36A-4889-A9D1-525CE6608181}">
   <dimension ref="A1:Z82"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,14 +1170,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27" t="s">
         <v>62</v>
       </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="28"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1027,6 +1264,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="H3" s="7" t="s">
@@ -1060,7 +1298,7 @@
       <c r="Z3" s="11"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="30">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1106,7 +1344,7 @@
       <c r="Z4" s="11"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="A5" s="30">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1148,7 +1386,7 @@
       <c r="Z5" s="11"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="30">
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1186,7 +1424,7 @@
       <c r="Z6" s="11"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="30">
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1220,7 +1458,7 @@
       <c r="Z7" s="11"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="30">
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -1276,7 +1514,7 @@
       <c r="Z8" s="11"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="H9" s="7" t="s">
@@ -1318,7 +1556,7 @@
       <c r="Z9" s="11"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1598,7 @@
       <c r="Z10" s="11"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="H11" s="7" t="s">
@@ -1398,7 +1636,7 @@
       <c r="Z11" s="11"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="30">
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1438,7 +1676,7 @@
       <c r="Z12" s="11"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="30">
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1490,7 +1728,7 @@
       <c r="Z13" s="11"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="30">
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1538,7 +1776,7 @@
       <c r="Z14" s="11"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="30">
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1584,7 +1822,7 @@
       <c r="Z15" s="11"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="31"/>
       <c r="H16" s="7" t="s">
         <v>15</v>
       </c>
@@ -1610,7 +1848,7 @@
       <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="5" t="s">
         <v>0</v>
       </c>
@@ -1656,6 +1894,7 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="29"/>
       <c r="H18" s="7" t="s">
         <v>17</v>
       </c>
@@ -1687,7 +1926,7 @@
       <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="A19" s="30">
         <v>10</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1724,7 +1963,7 @@
       <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+      <c r="A20" s="30">
         <v>11</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1761,7 +2000,7 @@
       <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="A21" s="30">
         <v>12</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1798,7 +2037,7 @@
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
+      <c r="A22" s="30">
         <v>13</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1835,7 +2074,7 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
+      <c r="A23" s="30">
         <v>14</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -1870,7 +2109,7 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="31"/>
       <c r="H24" s="7" t="s">
         <v>23</v>
       </c>
@@ -1898,7 +2137,7 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="3" t="s">
         <v>1</v>
       </c>
@@ -1927,6 +2166,7 @@
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
       <c r="H26" s="7" t="s">
         <v>29</v>
       </c>
@@ -1950,7 +2190,7 @@
       <c r="Z26" s="12"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
+      <c r="A27" s="30">
         <v>15</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1979,7 +2219,7 @@
       <c r="Z27" s="12"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
+      <c r="A28" s="30">
         <v>16</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -2008,7 +2248,7 @@
       <c r="Z28" s="12"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="A29" s="30">
         <v>17</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -2037,7 +2277,7 @@
       <c r="Z29" s="12"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="A30" s="30">
         <v>18</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -2066,6 +2306,7 @@
       <c r="Z30" s="12"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" s="29"/>
       <c r="H31" s="7" t="s">
         <v>34</v>
       </c>
@@ -2089,6 +2330,7 @@
       <c r="Z31" s="12"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
       <c r="H32" s="7" t="s">
         <v>35</v>
       </c>
@@ -2112,6 +2354,7 @@
       <c r="Z32" s="12"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="29"/>
       <c r="H33" s="7" t="s">
         <v>36</v>
       </c>
@@ -2135,6 +2378,7 @@
       <c r="Z33" s="12"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="29"/>
       <c r="H34" s="7" t="s">
         <v>37</v>
       </c>
@@ -2158,6 +2402,13 @@
       <c r="Z34" s="12"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
       <c r="H35" s="7" t="s">
         <v>38</v>
       </c>
@@ -2217,7 +2468,7 @@
         <v>67</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
@@ -2239,7 +2490,7 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B47" s="17" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
@@ -3473,15 +3724,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7F28C2-B0E0-4684-8294-C936A2350323}">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:G37"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
@@ -3493,14 +3744,14 @@
         <v>64</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="45" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="1"/>
@@ -3539,7 +3790,10 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+      <c r="B3" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="47"/>
       <c r="J3" s="7" t="s">
         <v>9</v>
       </c>
@@ -3567,8 +3821,11 @@
       <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>48</v>
+      <c r="B4" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>5</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>6</v>
@@ -3591,19 +3848,20 @@
       <c r="A5" s="14">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="7" t="s">
+      <c r="B5" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
@@ -3612,26 +3870,26 @@
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="7" t="s">
+      <c r="B6" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="J6" s="11"/>
       <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="L6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="11"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -3639,52 +3897,52 @@
       <c r="R6" s="11"/>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="7" t="s">
+      <c r="B7" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="J7" s="11"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="M7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="11"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="7" t="s">
+      <c r="B8" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="I8" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="N8" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="O8" s="11" t="s">
         <v>39</v>
       </c>
@@ -3700,26 +3958,23 @@
       <c r="S8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="T8" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="U8" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="T8" s="11"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" s="7" t="s">
+      <c r="B9" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="I9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="J9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
@@ -3729,24 +3984,27 @@
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J10" s="7" t="s">
+      <c r="B10" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="J10" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="K10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
@@ -3755,30 +4013,30 @@
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="7" t="s">
+      <c r="B11" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="J11" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="K11" s="11" t="s">
         <v>39</v>
       </c>
       <c r="L11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
@@ -3786,21 +4044,23 @@
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>9</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J12" s="7" t="s">
+      <c r="B12" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="J12" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="K12" s="11" t="s">
         <v>39</v>
       </c>
@@ -3810,34 +4070,32 @@
       <c r="M12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="N12" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="N12" s="11"/>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
       <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" s="7" t="s">
+      <c r="B13" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="48"/>
+      <c r="I13" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="J13" s="11"/>
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="N13" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="O13" s="11" t="s">
         <v>39</v>
       </c>
@@ -3850,25 +4108,22 @@
       <c r="R13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="S13" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="S13" s="11"/>
       <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>11</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="M14" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="N14" s="11" t="s">
         <v>39</v>
       </c>
@@ -3881,12 +4136,9 @@
       <c r="Q14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R14" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J15" s="7" t="s">
@@ -4026,7 +4278,9 @@
       <c r="U20" s="11"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
+      <c r="A21" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="J21" s="7" t="s">
         <v>20</v>
       </c>
@@ -4293,37 +4547,54 @@
       <c r="U35" s="12"/>
     </row>
     <row r="37" spans="6:21" ht="120" x14ac:dyDescent="0.25">
-      <c r="F37" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="G37" s="26" t="s">
-        <v>79</v>
+      <c r="F37" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B13:C13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A31A23-2872-4D60-AC2B-AF57F3740A38}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:AE79"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="17" max="18" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="B2" s="1"/>
       <c r="C2" s="7">
         <v>1</v>
@@ -4358,22 +4629,56 @@
       <c r="M2" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T2" s="1"/>
+      <c r="U2" s="7">
+        <v>1</v>
+      </c>
+      <c r="V2" s="7">
+        <v>2</v>
+      </c>
+      <c r="W2" s="7">
+        <v>3</v>
+      </c>
+      <c r="X2" s="7">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -4382,13 +4687,35 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -4400,14 +4727,30 @@
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -4418,15 +4761,31 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -4436,8 +4795,24 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
@@ -4445,7 +4820,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -4454,8 +4829,24 @@
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
@@ -4464,33 +4855,59 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE8" s="11"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -4502,16 +4919,32 @@
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -4522,19 +4955,37 @@
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -4544,22 +4995,42 @@
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="U11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -4568,8 +5039,30 @@
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="V12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="W12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="X12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
@@ -4578,24 +5071,48 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
@@ -4603,66 +5120,114 @@
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="T15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="X15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -4670,8 +5235,30 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="X16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
@@ -4681,25 +5268,51 @@
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE17" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>17</v>
       </c>
@@ -4710,14 +5323,30 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>18</v>
       </c>
@@ -4729,13 +5358,29 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
@@ -4748,13 +5393,28 @@
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
       <c r="K20" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
-      <c r="O20" s="2"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
@@ -4768,12 +5428,29 @@
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="18" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="M21" s="11"/>
       <c r="N21" s="2"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O21" s="1"/>
+      <c r="T21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE21" s="11"/>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>21</v>
       </c>
@@ -4785,19 +5462,53 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="M22" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="O22" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="P22" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q22" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R22" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE22" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>22</v>
       </c>
@@ -4810,16 +5521,46 @@
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
       <c r="K23" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="O23" s="41"/>
+      <c r="P23" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q23" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="R23" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE23" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>23</v>
       </c>
@@ -4833,13 +5574,41 @@
       <c r="J24" s="11"/>
       <c r="K24" s="11"/>
       <c r="L24" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="O24" s="41"/>
+      <c r="P24" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q24" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="R24" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE24" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>24</v>
       </c>
@@ -4854,10 +5623,36 @@
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
       <c r="M25" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="O25" s="42"/>
+      <c r="P25" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q25" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="R25" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>29</v>
       </c>
@@ -4872,8 +5667,22 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="12"/>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>30</v>
       </c>
@@ -4888,8 +5697,22 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="12"/>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>31</v>
       </c>
@@ -4904,8 +5727,22 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
+      <c r="AE28" s="12"/>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>32</v>
       </c>
@@ -4920,8 +5757,22 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="12"/>
+      <c r="AD29" s="12"/>
+      <c r="AE29" s="12"/>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
@@ -4936,8 +5787,22 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T30" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="12"/>
+      <c r="AD30" s="12"/>
+      <c r="AE30" s="12"/>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -4952,8 +5817,22 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="12"/>
+      <c r="Z31" s="12"/>
+      <c r="AA31" s="12"/>
+      <c r="AB31" s="12"/>
+      <c r="AC31" s="12"/>
+      <c r="AD31" s="12"/>
+      <c r="AE31" s="12"/>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>35</v>
       </c>
@@ -4968,8 +5847,22 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="T32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="12"/>
+      <c r="AA32" s="12"/>
+      <c r="AB32" s="12"/>
+      <c r="AC32" s="12"/>
+      <c r="AD32" s="12"/>
+      <c r="AE32" s="12"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -4984,8 +5877,22 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="T33" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="12"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12"/>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="12"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>37</v>
       </c>
@@ -5000,8 +5907,22 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="T34" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="12"/>
+      <c r="Y34" s="12"/>
+      <c r="Z34" s="12"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="12"/>
+      <c r="AD34" s="12"/>
+      <c r="AE34" s="12"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
         <v>38</v>
       </c>
@@ -5016,8 +5937,781 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
+      <c r="T35" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+      <c r="W35" s="12"/>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="12"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="12"/>
+      <c r="AC35" s="12"/>
+      <c r="AD35" s="12"/>
+      <c r="AE35" s="12"/>
+    </row>
+    <row r="40" spans="1:31" ht="105" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="O40" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="P40" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="D46" s="7">
+        <v>2</v>
+      </c>
+      <c r="E46" s="7">
+        <v>3</v>
+      </c>
+      <c r="F46" s="7">
+        <v>4</v>
+      </c>
+      <c r="G46" s="7">
+        <v>5</v>
+      </c>
+      <c r="H46" s="7">
+        <v>6</v>
+      </c>
+      <c r="I46" s="7">
+        <v>7</v>
+      </c>
+      <c r="J46" s="7">
+        <v>8</v>
+      </c>
+      <c r="K46" s="7">
+        <v>9</v>
+      </c>
+      <c r="L46" s="7">
+        <v>10</v>
+      </c>
+      <c r="M46" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J52" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="L52" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="M52" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I57" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="J57" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K57" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G58" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="H58" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="I58" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J58" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H59" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I59" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B61" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J61" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K61" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="L61" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="M61" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="11"/>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B64" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="L64" s="11"/>
+      <c r="M64" s="11"/>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B65" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="11"/>
+      <c r="L65" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="M65" s="11"/>
+      <c r="O65" s="1"/>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="K66" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="L66" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="M66" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="O66" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="P66" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q66" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="R66" s="34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B67" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="L67" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="M67" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O67" s="41"/>
+      <c r="P67" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q67" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="R67" s="35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B68" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="11"/>
+      <c r="L68" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M68" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="O68" s="41"/>
+      <c r="P68" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q68" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="R68" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B69" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="O69" s="42"/>
+      <c r="P69" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q69" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="R69" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="12"/>
+      <c r="M70" s="12"/>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B71" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="12"/>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B73" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="12"/>
+      <c r="K73" s="12"/>
+      <c r="L73" s="12"/>
+      <c r="M73" s="12"/>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B74" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
+      <c r="M74" s="12"/>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B75" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="12"/>
+      <c r="K75" s="12"/>
+      <c r="L75" s="12"/>
+      <c r="M75" s="12"/>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B76" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="12"/>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B77" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="12"/>
+      <c r="K77" s="12"/>
+      <c r="L77" s="12"/>
+      <c r="M77" s="12"/>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B78" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="12"/>
+      <c r="K78" s="12"/>
+      <c r="L78" s="12"/>
+      <c r="M78" s="12"/>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B79" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
+      <c r="L79" s="12"/>
+      <c r="M79" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="O66:O69"/>
+    <mergeCell ref="O22:O25"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>